<commit_message>
Docs: Update Excel templates with 10 new controls from gap analysis
- governance-maturity-dashboard.xlsx: Added all 10 new controls (1.20-1.22, 2.16-2.19, 3.10, 4.6-4.7), updated title to 58 controls, updated Summary Dashboard counts
- purview-administrator-checklist.xlsx: Added Control 1.22 Information Barriers
- sharepoint-administrator-checklist.xlsx: Added Controls 4.6, 4.7
- power-platform-administrator-checklist.xlsx: Added Controls 2.16, 2.17
- compliance-officer-checklist.xlsx: Added Controls 1.22, 2.18, 2.19, 3.10
- docs/downloads/index.md: Updated control assignments by role
- .claude/claude.md: Added Excel templates reference section
</commit_message>
<xml_diff>
--- a/docs/downloads/compliance-officer-checklist.xlsx
+++ b/docs/downloads/compliance-officer-checklist.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Checklist" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Checklist" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,6 +467,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
@@ -533,33 +534,31 @@
       <c r="E5" s="3" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>2.6</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>Model Risk Management (OCC 2011-12 / SR 11-7)</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="inlineStr">
-        <is>
-          <t>Not Started</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="inlineStr"/>
-      <c r="E6" s="3" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1.22</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Information Barriers for AI Agents</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>2.11</t>
+          <t>2.6</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Bias Testing and Fairness Assessment</t>
+          <t>Model Risk Management (OCC 2011-12 / SR 11-7)</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -573,12 +572,12 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>2.12</t>
+          <t>2.11</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>Supervision and Oversight (FINRA Rule 3110)</t>
+          <t>Bias Testing and Fairness Assessment</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -592,12 +591,12 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>2.13</t>
+          <t>2.12</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Documentation and Record Keeping</t>
+          <t>Supervision and Oversight (FINRA Rule 3110)</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -611,12 +610,12 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>2.13</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>Compliance and Regulatory Reporting</t>
+          <t>Documentation and Record Keeping</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -627,8 +626,80 @@
       <c r="D10" s="3" t="inlineStr"/>
       <c r="E10" s="3" t="inlineStr"/>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2.18</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Automated Conflict of Interest Testing</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2.19</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Customer AI Disclosure and Transparency</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+    </row>
     <row r="13">
-      <c r="A13" s="4" t="inlineStr">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>3.3</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Compliance and Regulatory Reporting</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="inlineStr"/>
+      <c r="E13" s="3" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>3.10</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Hallucination Feedback Loop</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+    </row>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17">
+      <c r="A17" s="4" t="inlineStr">
         <is>
           <t>FSI Agent Governance Framework v1.0 Beta</t>
         </is>

</xml_diff>

<commit_message>
Feat: v1.1.1 Researcher gap analysis response
Addresses findings from external researcher gap analysis.
Of 19 claimed gaps: 8 invalid (already covered), 5 partially valid
(minor enhancements), 2 valid (new content), 4 out of scope.

Added:
- Control 2.21: AI Marketing Claims and Substantiation (SEC Marketing Rule)
- 4 playbooks for Control 2.21
- SEC Marketing Rule section in regulatory-mappings.md

Enhanced (8 controls):
- 1.4: Copilot plugins/extensions terminology table
- 1.7: AI-generated communication tagging (FINRA 25-07)
- 1.8: AI-enabled threat patterns (deepfakes, AI phishing)
- 1.10: Monitored Copilot/AI locations table
- 1.11: PIM baselines for AI admin roles
- 1.23: PIM integration for sensitive agent operations
- 2.7: FSI-specific vendor categories (archiving vendors)
- 3.3: AI regulatory impact assessment template

Updated:
- Control count: 60 → 61
- CONTROL-INDEX.md, mkdocs.yml navigation
- Excel templates with new control
- Framework and reference documentation
</commit_message>
<xml_diff>
--- a/docs/downloads/compliance-officer-checklist.xlsx
+++ b/docs/downloads/compliance-officer-checklist.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,6 +467,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
@@ -660,43 +661,62 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="inlineStr">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2.21</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>AI Marketing Claims and Substantiation</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
         <is>
           <t>3.3</t>
         </is>
       </c>
-      <c r="B13" s="3" t="inlineStr">
+      <c r="B14" s="3" t="inlineStr">
         <is>
           <t>Compliance and Regulatory Reporting</t>
         </is>
       </c>
-      <c r="C13" s="3" t="inlineStr">
-        <is>
-          <t>Not Started</t>
-        </is>
-      </c>
-      <c r="D13" s="3" t="inlineStr"/>
-      <c r="E13" s="3" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="inlineStr"/>
+      <c r="E14" s="3" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
         <is>
           <t>3.10</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Hallucination Feedback Loop</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Not Started</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="inlineStr">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+    </row>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18">
+      <c r="A18" s="4" t="inlineStr">
         <is>
           <t>FSI Agent Governance Framework v1.1</t>
         </is>

</xml_diff>